<commit_message>
qubee v0.8.1 final draft
</commit_message>
<xml_diff>
--- a/media/supported_onnx.xlsx
+++ b/media/supported_onnx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jinman\Desktop\workspace\Manual\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{631B2DF8-E300-4F80-977A-3ABD07ABEB1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AC6B492-AE0D-4038-A818-B8D6A82F0ACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{82FA91C1-AFA3-4631-B311-4F4CA060295C}"/>
+    <workbookView xWindow="10620" yWindow="1800" windowWidth="17610" windowHeight="11295" xr2:uid="{82FA91C1-AFA3-4631-B311-4F4CA060295C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -815,8 +815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{456629B3-8544-4598-9B44-E584E1332484}">
   <dimension ref="A1:B76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>